<commit_message>
adding updates to admin pages
</commit_message>
<xml_diff>
--- a/Testing Script.xlsx
+++ b/Testing Script.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rache\Documents\sky-git-team2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D11DB155-6E5E-40B1-8152-16280929B47C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E00CCDA-9FA4-42BE-BA35-48C5D0582285}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4000" yWindow="1830" windowWidth="14400" windowHeight="7280" xr2:uid="{F029CBA5-67CE-431B-AFF4-8D9EE2FC63BA}"/>
+    <workbookView xWindow="28680" yWindow="690" windowWidth="19440" windowHeight="14880" xr2:uid="{F029CBA5-67CE-431B-AFF4-8D9EE2FC63BA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="18">
   <si>
     <t>register someone new</t>
   </si>
@@ -36,9 +36,6 @@
     <t>check added to data base in credential</t>
   </si>
   <si>
-    <t>log in as new person</t>
-  </si>
-  <si>
     <t>log out</t>
   </si>
   <si>
@@ -51,10 +48,37 @@
     <t>update-customer - do address for ease</t>
   </si>
   <si>
-    <t>no</t>
-  </si>
-  <si>
     <t>register-pet</t>
+  </si>
+  <si>
+    <t>log in as admin</t>
+  </si>
+  <si>
+    <t>log in as that new person</t>
+  </si>
+  <si>
+    <t>update-password back to 'password'</t>
+  </si>
+  <si>
+    <t>update-pet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">from admin page open each table option </t>
+  </si>
+  <si>
+    <t>for each table click through to a record and update something</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>check in db</t>
+  </si>
+  <si>
+    <t>logout</t>
+  </si>
+  <si>
+    <t>login</t>
   </si>
 </sst>
 </file>
@@ -90,8 +114,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -406,67 +431,142 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADB9AA93-DEDA-4691-91C9-9A3362145F9E}">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:B17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="20.1796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="54" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B1" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B2" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B3" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
+      <c r="B5" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
+      <c r="B6" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
+      <c r="B9" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
         <v>7</v>
       </c>
-      <c r="D7" t="s">
+      <c r="B13" s="1"/>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>11</v>
+      </c>
+      <c r="B14" s="1"/>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>6</v>
-      </c>
-      <c r="D8" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>9</v>
-      </c>
+      <c r="B15" s="1"/>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>12</v>
+      </c>
+      <c r="B16" s="1"/>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>13</v>
+      </c>
+      <c r="B17" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>